<commit_message>
Update Output Excel File
</commit_message>
<xml_diff>
--- a/Excel VBA x UiPath/Column Width AutoFit/Output/SampleData.xlsx
+++ b/Excel VBA x UiPath/Column Width AutoFit/Output/SampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath_RPA\VBA_with_RPA\Column_Width_AutoFit\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA_UiPath\Excel VBA x RPA\Column Width AutoFit\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
-    <sheet name="工作表2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Column1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,75 +56,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ABCDEFGH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IJKLMNO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PQRST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UVW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XYZ</t>
+    <t>ABCDEFGHIJKLMNOP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QRSTUVWXY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZABC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEFGH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IJKLMNOPQRST</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Column4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Column5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Column6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>G</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>J</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AAABAC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADAEAFAGAH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AJAK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ALAMAN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -179,7 +130,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -188,6 +139,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,20 +424,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="工作表1"/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -493,10 +448,13 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -504,10 +462,13 @@
         <v>8</v>
       </c>
       <c r="C2" s="1">
-        <v>12345</v>
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1234567</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -515,10 +476,13 @@
         <v>9</v>
       </c>
       <c r="C3" s="1">
-        <v>6789</v>
+        <v>234567890</v>
+      </c>
+      <c r="D3" s="3">
+        <v>89012345</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -526,10 +490,13 @@
         <v>10</v>
       </c>
       <c r="C4" s="1">
-        <v>123</v>
+        <v>1234</v>
+      </c>
+      <c r="D4" s="1">
+        <v>678</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -537,10 +504,13 @@
         <v>11</v>
       </c>
       <c r="C5" s="1">
-        <v>456789</v>
+        <v>56789012345</v>
+      </c>
+      <c r="D5" s="3">
+        <v>90123</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -548,98 +518,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="1">
-        <v>12345678901</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="工作表2"/>
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="1">
-        <v>23456</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1">
-        <v>78900</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="1">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="1">
-        <v>123</v>
+        <v>67890</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4567890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>